<commit_message>
fin script db + début interface graphique
ajouts de plusieurs exemples dans le projet afin de m'aider.
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>création des scénarios et maquettes</t>
+  </si>
+  <si>
+    <t>refonte du mcd+mld</t>
+  </si>
+  <si>
+    <t>recherches pour le choix entre MySQL ou SQLite, avantages/désaventages et les besoins nécessaires.</t>
+  </si>
+  <si>
+    <t>.02.2019</t>
   </si>
 </sst>
 </file>
@@ -282,15 +291,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E40" totalsRowShown="0">
-  <autoFilter ref="A1:E40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E46" totalsRowShown="0">
+  <autoFilter ref="A1:E46"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="4"/>
     <tableColumn id="5" name="Type" dataDxfId="3"/>
     <tableColumn id="2" name="Activité" dataDxfId="2"/>
     <tableColumn id="3" name="Temps" dataDxfId="1"/>
     <tableColumn id="4" name="Temps journée" dataDxfId="0">
-      <calculatedColumnFormula>SUM($D2:$D$40)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM($D2:$D$46)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
@@ -561,10 +570,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,83 +774,221 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
+      <c r="A15" s="12">
+        <v>43507</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUM($D$10:$D16)</f>
+        <v>0.21874999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUM($D$10:$D17)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <f>SUM($D$10:$D19)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <f>SUM($D$10:$D20)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <f>SUM($D$10:$D21)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <f>SUM($D$10:$D22)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <f>SUM($D$10:$D23)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <f>SUM($D$10:$D24)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <f>SUM($D$10:$D25)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="1">
+        <f>SUM($D$10:$D26)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <f>SUM($D$10:$D27)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="1">
+        <f>SUM($D$10:$D28)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <f>SUM($D$10:$D29)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <f>SUM($D$10:$D30)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <f>SUM($D$10:$D31)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <f>SUM($D$10:$D32)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <f>SUM($D$10:$D33)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="1"/>
+      <c r="E34" s="1">
+        <f>SUM($D$10:$D34)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <f>SUM($D$10:$D35)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <f>SUM($D$10:$D36)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37" s="1"/>
+      <c r="E37" s="1">
+        <f>SUM($D$10:$D37)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38" s="1"/>
+      <c r="E38" s="1">
+        <f>SUM($D$10:$D38)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="1"/>
+      <c r="E39" s="1">
+        <f>SUM($D$10:$D39)</f>
+        <v>0.27083333333333331</v>
+      </c>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E40" s="1"/>
+      <c r="E40" s="1">
+        <f>SUM($D$10:$D40)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <f>SUM($D$10:$D41)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <f>SUM($D$10:$D42)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <f>SUM($D$10:$D43)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <f>SUM($D$10:$D44)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <f>SUM($D$10:$D45)</f>
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <f>SUM($D$10:$D46)</f>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -856,7 +1003,7 @@
           <x14:formula1>
             <xm:f>Parametre!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B2940</xm:sqref>
+          <xm:sqref>B2:B2946</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
bug lors du push... mes fichiers se sont corrompu
je refais l'interface + le code
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -88,7 +88,7 @@
     <t>recherches pour le choix entre MySQL ou SQLite, avantages/désaventages et les besoins nécessaires.</t>
   </si>
   <si>
-    <t>.02.2019</t>
+    <t>problèmes avec visual studio, j'ai du réinstaller tout le programme</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,8 +813,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>22</v>
+      <c r="A18" s="12">
+        <v>43509</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -822,6 +822,12 @@
       <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="1">
         <f>SUM($D$10:$D19)</f>
         <v>0.27083333333333331</v>

</xml_diff>

<commit_message>
création d'une IA beaucoup plus intelligente
correction du fait que l'IA mettais ses "O" sur nos "X"
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>début de l'intelligence artificielle de niveau moyen</t>
+  </si>
+  <si>
+    <t>j'avais un bug dans ma manière de vérifier les cases, je cherchais un moyen autre moyen de faire mon idée</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,12 +1166,21 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="1">
-        <f>SUM($D$10:$D42)</f>
-        <v>0.90972222222222199</v>
-      </c>
+      <c r="A42" s="12">
+        <v>43502</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="E43" s="1">
         <f>SUM($D$10:$D43)</f>
         <v>0.90972222222222199</v>

</xml_diff>

<commit_message>
avancement dans la doc
ia niveau moyen terminée, début des test pour voir si elle plante
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>début de la création de la planif. Initiale</t>
-  </si>
-  <si>
-    <t>Total -&gt;</t>
   </si>
   <si>
     <t>continuation de la planification et début de la documentation</t>
@@ -138,6 +135,12 @@
   </si>
   <si>
     <t>implémentation d'une IA plus intelligente</t>
+  </si>
+  <si>
+    <t>Documentation, refonte des scénarios</t>
+  </si>
+  <si>
+    <t>001:30:00</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -288,7 +291,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -340,15 +342,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E46" totalsRowShown="0">
-  <autoFilter ref="A1:E46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E124" totalsRowShown="0">
+  <autoFilter ref="A1:E124"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="4"/>
     <tableColumn id="5" name="Type" dataDxfId="3"/>
     <tableColumn id="2" name="Activité" dataDxfId="2"/>
     <tableColumn id="3" name="Temps" dataDxfId="1"/>
     <tableColumn id="4" name="Temps journée" dataDxfId="0">
-      <calculatedColumnFormula>SUM($D2:$D$46)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM($D2:$D$124)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
@@ -619,10 +621,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,25 +661,21 @@
       <c r="C2" s="9"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="G2" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="19">
-        <v>0.2048611111111111</v>
-      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="11">
         <v>6.25E-2</v>
       </c>
       <c r="E3" s="1">
-        <f>SUM($D3:$D$3)</f>
+        <f>SUM($D$3:$D3)</f>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -688,21 +686,21 @@
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E5" s="1">
-        <f>SUM($D$5:$D5)</f>
-        <v>3.125E-2</v>
+        <f>SUM($D$3:$D5)</f>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -712,36 +710,36 @@
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>14</v>
+      <c r="C7" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="E7" s="1">
-        <f>SUM($D$7:$D7)</f>
-        <v>4.8611111111111112E-2</v>
+        <f>SUM($D$3:$D7)</f>
+        <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>15</v>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E8" s="1">
-        <f>SUM($D$7:$D8)</f>
-        <v>6.25E-2</v>
+        <f>SUM($D$3:$D8)</f>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -751,21 +749,21 @@
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>16</v>
+      <c r="C10" s="19" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E10" s="1">
-        <f>SUM($D$10:$D10)</f>
-        <v>8.3333333333333329E-2</v>
+        <f>SUM($D$3:$D10)</f>
+        <v>0.23958333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -775,21 +773,21 @@
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>17</v>
+      <c r="C12" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="D12" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E12" s="1">
-        <f>SUM($D$10:$D12)</f>
-        <v>0.11458333333333333</v>
+        <f>SUM($D$3:$D12)</f>
+        <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -797,14 +795,14 @@
         <v>7</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E13" s="1">
-        <f>SUM($D$10:$D13)</f>
-        <v>0.14583333333333331</v>
+        <f>SUM($D$3:$D13)</f>
+        <v>0.30208333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -812,14 +810,14 @@
         <v>9</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="E14" s="1">
-        <f>SUM($D$10:$D14)</f>
-        <v>0.20833333333333331</v>
+        <f>SUM($D$3:$D14)</f>
+        <v>0.36458333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -836,14 +834,14 @@
         <v>7</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E16" s="1">
-        <f>SUM($D$10:$D16)</f>
-        <v>0.21874999999999997</v>
+        <f>SUM($D$3:$D16)</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,14 +849,14 @@
         <v>5</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="2">
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="E17" s="1">
-        <f>SUM($D$10:$D17)</f>
-        <v>0.27083333333333331</v>
+        <f>SUM($D$3:$D17)</f>
+        <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -875,14 +873,14 @@
         <v>7</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E19" s="1">
-        <f>SUM($D$10:$D19)</f>
-        <v>0.30208333333333331</v>
+        <f>SUM($D$3:$D19)</f>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -890,14 +888,14 @@
         <v>5</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E20" s="1">
-        <f>SUM($D$10:$D20)</f>
-        <v>0.33333333333333331</v>
+        <f>SUM($D$3:$D20)</f>
+        <v>0.48958333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -914,14 +912,14 @@
         <v>7</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E22" s="1">
-        <f>SUM($D$10:$D22)</f>
-        <v>0.36458333333333331</v>
+        <f>SUM($D$3:$D22)</f>
+        <v>0.52083333333333326</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -938,14 +936,14 @@
         <v>7</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="2">
         <v>0.17708333333333334</v>
       </c>
       <c r="E24" s="1">
-        <f>SUM($D$10:$D24)</f>
-        <v>0.54166666666666663</v>
+        <f>SUM($D$3:$D24)</f>
+        <v>0.69791666666666663</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -962,14 +960,14 @@
         <v>7</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E26" s="1">
-        <f>SUM($D$10:$D26)</f>
-        <v>0.55555555555555547</v>
+        <f>SUM($D$3:$D26)</f>
+        <v>0.71180555555555547</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -977,14 +975,14 @@
         <v>7</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E27" s="1">
-        <f>SUM($D$10:$D27)</f>
-        <v>0.5972222222222221</v>
+        <f>SUM($D$3:$D27)</f>
+        <v>0.7534722222222221</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,14 +999,14 @@
         <v>9</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E29" s="1">
-        <f>SUM($D$10:$D29)</f>
-        <v>0.6284722222222221</v>
+        <f>SUM($D$3:$D29)</f>
+        <v>0.7847222222222221</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1016,14 +1014,14 @@
         <v>7</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E30" s="1">
-        <f>SUM($D$10:$D30)</f>
-        <v>0.6597222222222221</v>
+        <f>SUM($D$3:$D30)</f>
+        <v>0.8159722222222221</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1040,14 +1038,14 @@
         <v>7</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="E32" s="1">
-        <f>SUM($D$10:$D32)</f>
-        <v>0.7222222222222221</v>
+        <f>SUM($D$3:$D32)</f>
+        <v>0.8784722222222221</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,14 +1062,14 @@
         <v>7</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="E34" s="1">
-        <f>SUM($D$10:$D34)</f>
-        <v>0.7847222222222221</v>
+        <f>SUM($D$3:$D34)</f>
+        <v>0.9409722222222221</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1088,14 +1086,14 @@
         <v>7</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="E36" s="1">
-        <f>SUM($D$10:$D36)</f>
-        <v>0.8472222222222221</v>
+        <f>SUM($D$3:$D36)</f>
+        <v>1.0034722222222221</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1112,14 +1110,14 @@
         <v>7</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E38" s="1">
-        <f>SUM($D$10:$D38)</f>
-        <v>0.8784722222222221</v>
+        <f>SUM($D$3:$D38)</f>
+        <v>1.0347222222222221</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,14 +1125,14 @@
         <v>7</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="E39" s="1">
-        <f>SUM($D$10:$D39)</f>
-        <v>0.89236111111111094</v>
+        <f>SUM($D$3:$D39)</f>
+        <v>1.0486111111111109</v>
       </c>
       <c r="F39" s="7"/>
     </row>
@@ -1143,14 +1141,14 @@
         <v>7</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="2">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="E40" s="1">
-        <f>SUM($D$10:$D40)</f>
-        <v>0.90277777777777757</v>
+        <f>SUM($D$3:$D40)</f>
+        <v>1.0590277777777777</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1158,14 +1156,14 @@
         <v>7</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" s="2">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E41" s="1">
-        <f>SUM($D$10:$D41)</f>
-        <v>0.90972222222222199</v>
+        <f>SUM($D$3:$D41)</f>
+        <v>1.0659722222222221</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,14 +1180,14 @@
         <v>5</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" s="2">
         <v>3.125E-2</v>
       </c>
       <c r="E43" s="1">
-        <f>SUM($D$10:$D43)</f>
-        <v>0.94097222222222199</v>
+        <f>SUM($D$3:$D43)</f>
+        <v>1.0972222222222221</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,26 +1195,506 @@
         <v>7</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" s="2">
         <v>6.25E-2</v>
       </c>
       <c r="E44" s="1">
-        <f>SUM($D$10:$D44)</f>
-        <v>1.0034722222222219</v>
+        <f>SUM($D$3:$D44)</f>
+        <v>1.1597222222222221</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E45" s="1">
-        <f>SUM($D$10:$D45)</f>
-        <v>1.0034722222222219</v>
-      </c>
+      <c r="A45" s="12">
+        <v>43503</v>
+      </c>
+      <c r="B45" s="12"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E46" s="1">
-        <f>SUM($D$10:$D46)</f>
-        <v>1.0034722222222219</v>
+        <f>SUM($D$3:$D46)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <f>SUM($D$3:$D47)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <f>SUM($D$3:$D48)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <f>SUM($D$3:$D49)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <f>SUM($D$3:$D50)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <f>SUM($D$3:$D51)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <f>SUM($D$3:$D52)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <f>SUM($D$3:$D53)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <f>SUM($D$3:$D54)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <f>SUM($D$3:$D55)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <f>SUM($D$3:$D56)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <f>SUM($D$3:$D57)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <f>SUM($D$3:$D58)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <f>SUM($D$3:$D59)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <f>SUM($D$3:$D60)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="1">
+        <f>SUM($D$3:$D61)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="1">
+        <f>SUM($D$3:$D62)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="1">
+        <f>SUM($D$3:$D63)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="1">
+        <f>SUM($D$3:$D64)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="1">
+        <f>SUM($D$3:$D65)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="1">
+        <f>SUM($D$3:$D66)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="1">
+        <f>SUM($D$3:$D67)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="1">
+        <f>SUM($D$3:$D68)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="1">
+        <f>SUM($D$3:$D69)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="1">
+        <f>SUM($D$3:$D70)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="1">
+        <f>SUM($D$3:$D71)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="1">
+        <f>SUM($D$3:$D72)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="1">
+        <f>SUM($D$3:$D73)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
+        <f>SUM($D$3:$D74)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="1">
+        <f>SUM($D$3:$D75)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
+        <f>SUM($D$3:$D76)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="1">
+        <f>SUM($D$3:$D77)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="1">
+        <f>SUM($D$3:$D78)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="1">
+        <f>SUM($D$3:$D79)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="1">
+        <f>SUM($D$3:$D80)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="1">
+        <f>SUM($D$3:$D81)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="1">
+        <f>SUM($D$3:$D82)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="1">
+        <f>SUM($D$3:$D83)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="1">
+        <f>SUM($D$3:$D84)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="1">
+        <f>SUM($D$3:$D85)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="1">
+        <f>SUM($D$3:$D86)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="1">
+        <f>SUM($D$3:$D87)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="1">
+        <f>SUM($D$3:$D88)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="1">
+        <f>SUM($D$3:$D89)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="1">
+        <f>SUM($D$3:$D90)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="1">
+        <f>SUM($D$3:$D91)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="1">
+        <f>SUM($D$3:$D92)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="1">
+        <f>SUM($D$3:$D93)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="1">
+        <f>SUM($D$3:$D94)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="1">
+        <f>SUM($D$3:$D95)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="1">
+        <f>SUM($D$3:$D96)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="1">
+        <f>SUM($D$3:$D97)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="1">
+        <f>SUM($D$3:$D98)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="1">
+        <f>SUM($D$3:$D99)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="1">
+        <f>SUM($D$3:$D100)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="1">
+        <f>SUM($D$3:$D101)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="1">
+        <f>SUM($D$3:$D102)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="1">
+        <f>SUM($D$3:$D103)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="1">
+        <f>SUM($D$3:$D104)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="1">
+        <f>SUM($D$3:$D105)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="1">
+        <f>SUM($D$3:$D106)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="1">
+        <f>SUM($D$3:$D107)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="1">
+        <f>SUM($D$3:$D108)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="1">
+        <f>SUM($D$3:$D109)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="1">
+        <f>SUM($D$3:$D110)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="1">
+        <f>SUM($D$3:$D111)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="1">
+        <f>SUM($D$3:$D112)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="1">
+        <f>SUM($D$3:$D113)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="1">
+        <f>SUM($D$3:$D114)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="1">
+        <f>SUM($D$3:$D115)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="1">
+        <f>SUM($D$3:$D116)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="1">
+        <f>SUM($D$3:$D117)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="1">
+        <f>SUM($D$3:$D118)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="1">
+        <f>SUM($D$3:$D119)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="1">
+        <f>SUM($D$3:$D120)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="1">
+        <f>SUM($D$3:$D121)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="1">
+        <f>SUM($D$3:$D122)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="1">
+        <f>SUM($D$3:$D123)</f>
+        <v>1.1597222222222221</v>
+      </c>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="1">
+        <f>SUM($D$3:$D124)</f>
+        <v>1.1597222222222221</v>
       </c>
     </row>
   </sheetData>
@@ -1251,32 +1729,32 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
j'ai terminé la gestion des parties locales en solo et multijoueur
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>la requête s'envoie enfin de manière correcte</t>
+  </si>
+  <si>
+    <t>après avoir ajouté la base de données, de manière inexpliquée mon jeu ne répond plus</t>
+  </si>
+  <si>
+    <t>correction des bugs, enregistrement des scores + suppression et centrage de toute les fenêtres</t>
   </si>
 </sst>
 </file>
@@ -642,7 +648,7 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,7 +1324,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
-        <v>43506</v>
+        <v>43507</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="13"/>
@@ -1371,417 +1377,441 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="1">
-        <f>SUM($D$3:$D56)</f>
-        <v>1.5069444444444442</v>
-      </c>
+      <c r="A56" s="12">
+        <v>43508</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E57" s="1">
         <f>SUM($D$3:$D57)</f>
-        <v>1.5069444444444442</v>
+        <v>1.5694444444444442</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="1">
-        <f>SUM($D$3:$D58)</f>
-        <v>1.5069444444444442</v>
-      </c>
+      <c r="A58" s="12">
+        <v>43509</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E59" s="1">
         <f>SUM($D$3:$D59)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E60" s="1">
         <f>SUM($D$3:$D60)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E61" s="1">
         <f>SUM($D$3:$D61)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E62" s="1">
         <f>SUM($D$3:$D62)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E63" s="1">
         <f>SUM($D$3:$D63)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E64" s="1">
         <f>SUM($D$3:$D64)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="1">
         <f>SUM($D$3:$D65)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="1">
         <f>SUM($D$3:$D66)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" s="1">
         <f>SUM($D$3:$D67)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" s="1">
         <f>SUM($D$3:$D68)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" s="1">
         <f>SUM($D$3:$D69)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="1">
         <f>SUM($D$3:$D70)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="1">
         <f>SUM($D$3:$D71)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72" s="1">
         <f>SUM($D$3:$D72)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="73" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E73" s="1">
         <f>SUM($D$3:$D73)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="74" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E74" s="1">
         <f>SUM($D$3:$D74)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="75" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E75" s="1">
         <f>SUM($D$3:$D75)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="76" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E76" s="1">
         <f>SUM($D$3:$D76)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="77" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E77" s="1">
         <f>SUM($D$3:$D77)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="78" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E78" s="1">
         <f>SUM($D$3:$D78)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="79" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E79" s="1">
         <f>SUM($D$3:$D79)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="80" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E80" s="1">
         <f>SUM($D$3:$D80)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="1">
         <f>SUM($D$3:$D81)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="1">
         <f>SUM($D$3:$D82)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="1">
         <f>SUM($D$3:$D83)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="1">
         <f>SUM($D$3:$D84)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="1">
         <f>SUM($D$3:$D85)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" s="1">
         <f>SUM($D$3:$D86)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" s="1">
         <f>SUM($D$3:$D87)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" s="1">
         <f>SUM($D$3:$D88)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" s="1">
         <f>SUM($D$3:$D89)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" s="1">
         <f>SUM($D$3:$D90)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" s="1">
         <f>SUM($D$3:$D91)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" s="1">
         <f>SUM($D$3:$D92)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" s="1">
         <f>SUM($D$3:$D93)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" s="1">
         <f>SUM($D$3:$D94)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" s="1">
         <f>SUM($D$3:$D95)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="1">
         <f>SUM($D$3:$D96)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="1">
         <f>SUM($D$3:$D97)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="1">
         <f>SUM($D$3:$D98)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="1">
         <f>SUM($D$3:$D99)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="1">
         <f>SUM($D$3:$D100)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="1">
         <f>SUM($D$3:$D101)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="1">
         <f>SUM($D$3:$D102)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="1">
         <f>SUM($D$3:$D103)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="1">
         <f>SUM($D$3:$D104)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="1">
         <f>SUM($D$3:$D105)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="1">
         <f>SUM($D$3:$D106)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="1">
         <f>SUM($D$3:$D107)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="1">
         <f>SUM($D$3:$D108)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="1">
         <f>SUM($D$3:$D109)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="1">
         <f>SUM($D$3:$D110)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="1">
         <f>SUM($D$3:$D111)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="1">
         <f>SUM($D$3:$D112)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="1">
         <f>SUM($D$3:$D113)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="1">
         <f>SUM($D$3:$D114)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="1">
         <f>SUM($D$3:$D115)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="1">
         <f>SUM($D$3:$D116)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="1">
         <f>SUM($D$3:$D117)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="1">
         <f>SUM($D$3:$D118)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="1">
         <f>SUM($D$3:$D119)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="1">
         <f>SUM($D$3:$D120)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="1">
         <f>SUM($D$3:$D121)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="1">
         <f>SUM($D$3:$D122)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="1">
         <f>SUM($D$3:$D123)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="1">
         <f>SUM($D$3:$D124)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6319444444444442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
toute la documentation pour la première partie est faite à 80%
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>correction des bugs, enregistrement des scores + suppression et centrage de toute les fenêtres</t>
+  </si>
+  <si>
+    <t>j'ai refait plusieurs points dans la doc et je refais la partie implémentation</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,393 +1428,405 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="1">
-        <f>SUM($D$3:$D60)</f>
-        <v>1.6319444444444442</v>
-      </c>
+      <c r="A60" s="12">
+        <v>43510</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="2">
+        <v>9.375E-2</v>
+      </c>
       <c r="E61" s="1">
         <f>SUM($D$3:$D61)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E62" s="1">
         <f>SUM($D$3:$D62)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E63" s="1">
         <f>SUM($D$3:$D63)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E64" s="1">
         <f>SUM($D$3:$D64)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="1">
         <f>SUM($D$3:$D65)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="1">
         <f>SUM($D$3:$D66)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" s="1">
         <f>SUM($D$3:$D67)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" s="1">
         <f>SUM($D$3:$D68)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" s="1">
         <f>SUM($D$3:$D69)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="1">
         <f>SUM($D$3:$D70)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="1">
         <f>SUM($D$3:$D71)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72" s="1">
         <f>SUM($D$3:$D72)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="73" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E73" s="1">
         <f>SUM($D$3:$D73)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="74" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E74" s="1">
         <f>SUM($D$3:$D74)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="75" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E75" s="1">
         <f>SUM($D$3:$D75)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="76" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E76" s="1">
         <f>SUM($D$3:$D76)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="77" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E77" s="1">
         <f>SUM($D$3:$D77)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="78" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E78" s="1">
         <f>SUM($D$3:$D78)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="79" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E79" s="1">
         <f>SUM($D$3:$D79)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="80" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E80" s="1">
         <f>SUM($D$3:$D80)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="1">
         <f>SUM($D$3:$D81)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="1">
         <f>SUM($D$3:$D82)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="1">
         <f>SUM($D$3:$D83)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="1">
         <f>SUM($D$3:$D84)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="1">
         <f>SUM($D$3:$D85)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" s="1">
         <f>SUM($D$3:$D86)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" s="1">
         <f>SUM($D$3:$D87)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" s="1">
         <f>SUM($D$3:$D88)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" s="1">
         <f>SUM($D$3:$D89)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" s="1">
         <f>SUM($D$3:$D90)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" s="1">
         <f>SUM($D$3:$D91)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" s="1">
         <f>SUM($D$3:$D92)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" s="1">
         <f>SUM($D$3:$D93)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" s="1">
         <f>SUM($D$3:$D94)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" s="1">
         <f>SUM($D$3:$D95)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="1">
         <f>SUM($D$3:$D96)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="1">
         <f>SUM($D$3:$D97)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="1">
         <f>SUM($D$3:$D98)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="1">
         <f>SUM($D$3:$D99)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="1">
         <f>SUM($D$3:$D100)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="1">
         <f>SUM($D$3:$D101)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="1">
         <f>SUM($D$3:$D102)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="1">
         <f>SUM($D$3:$D103)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="1">
         <f>SUM($D$3:$D104)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="1">
         <f>SUM($D$3:$D105)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="1">
         <f>SUM($D$3:$D106)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="1">
         <f>SUM($D$3:$D107)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="1">
         <f>SUM($D$3:$D108)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="1">
         <f>SUM($D$3:$D109)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="1">
         <f>SUM($D$3:$D110)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="1">
         <f>SUM($D$3:$D111)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="1">
         <f>SUM($D$3:$D112)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="1">
         <f>SUM($D$3:$D113)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="1">
         <f>SUM($D$3:$D114)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="1">
         <f>SUM($D$3:$D115)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="1">
         <f>SUM($D$3:$D116)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="1">
         <f>SUM($D$3:$D117)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="1">
         <f>SUM($D$3:$D118)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="1">
         <f>SUM($D$3:$D119)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="1">
         <f>SUM($D$3:$D120)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="1">
         <f>SUM($D$3:$D121)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="1">
         <f>SUM($D$3:$D122)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="1">
         <f>SUM($D$3:$D123)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="1">
         <f>SUM($D$3:$D124)</f>
-        <v>1.6319444444444442</v>
+        <v>1.7256944444444442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction liées aux boutons, doxygen crée
avancement de la documentation et jdt
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>correction des test suite à un changement dans la classe database</t>
+  </si>
+  <si>
+    <t>j'ai effectué la pop-up message, début de la page informations</t>
+  </si>
+  <si>
+    <t>j'ai terminé toutes les pages</t>
   </si>
 </sst>
 </file>
@@ -657,7 +663,7 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,364 +1502,388 @@
         <v>1.9444444444444442</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="1">
-        <f>SUM($D$3:$D65)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="12">
+        <v>43541</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E66" s="1">
         <f>SUM($D$3:$D66)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="1">
-        <f>SUM($D$3:$D67)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0069444444444442</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="12">
+        <v>43542</v>
+      </c>
+      <c r="B67" s="12"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E68" s="1">
         <f>SUM($D$3:$D68)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E69" s="1">
         <f>SUM($D$3:$D69)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E70" s="1">
         <f>SUM($D$3:$D70)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E71" s="1">
         <f>SUM($D$3:$D71)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E72" s="1">
         <f>SUM($D$3:$D72)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E73" s="1">
         <f>SUM($D$3:$D73)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E74" s="1">
         <f>SUM($D$3:$D74)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E75" s="1">
         <f>SUM($D$3:$D75)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E76" s="1">
         <f>SUM($D$3:$D76)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E77" s="1">
         <f>SUM($D$3:$D77)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E78" s="1">
         <f>SUM($D$3:$D78)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E79" s="1">
         <f>SUM($D$3:$D79)</f>
-        <v>1.9444444444444442</v>
-      </c>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+        <v>2.0694444444444442</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E80" s="1">
         <f>SUM($D$3:$D80)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="1">
         <f>SUM($D$3:$D81)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="1">
         <f>SUM($D$3:$D82)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="1">
         <f>SUM($D$3:$D83)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="1">
         <f>SUM($D$3:$D84)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="1">
         <f>SUM($D$3:$D85)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" s="1">
         <f>SUM($D$3:$D86)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" s="1">
         <f>SUM($D$3:$D87)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" s="1">
         <f>SUM($D$3:$D88)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" s="1">
         <f>SUM($D$3:$D89)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" s="1">
         <f>SUM($D$3:$D90)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" s="1">
         <f>SUM($D$3:$D91)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" s="1">
         <f>SUM($D$3:$D92)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" s="1">
         <f>SUM($D$3:$D93)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" s="1">
         <f>SUM($D$3:$D94)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" s="1">
         <f>SUM($D$3:$D95)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="1">
         <f>SUM($D$3:$D96)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="1">
         <f>SUM($D$3:$D97)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="1">
         <f>SUM($D$3:$D98)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="1">
         <f>SUM($D$3:$D99)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="1">
         <f>SUM($D$3:$D100)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="1">
         <f>SUM($D$3:$D101)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="1">
         <f>SUM($D$3:$D102)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="1">
         <f>SUM($D$3:$D103)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="1">
         <f>SUM($D$3:$D104)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="1">
         <f>SUM($D$3:$D105)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="1">
         <f>SUM($D$3:$D106)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="1">
         <f>SUM($D$3:$D107)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="1">
         <f>SUM($D$3:$D108)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="1">
         <f>SUM($D$3:$D109)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="1">
         <f>SUM($D$3:$D110)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="1">
         <f>SUM($D$3:$D111)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="1">
         <f>SUM($D$3:$D112)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="1">
         <f>SUM($D$3:$D113)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="1">
         <f>SUM($D$3:$D114)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="1">
         <f>SUM($D$3:$D115)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="1">
         <f>SUM($D$3:$D116)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="1">
         <f>SUM($D$3:$D117)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="1">
         <f>SUM($D$3:$D118)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="1">
         <f>SUM($D$3:$D119)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="1">
         <f>SUM($D$3:$D120)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="1">
         <f>SUM($D$3:$D121)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="1">
         <f>SUM($D$3:$D122)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="1">
         <f>SUM($D$3:$D123)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="1">
         <f>SUM($D$3:$D124)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0694444444444442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
début des test réseau, je n'arrive pas a fermer le form
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>génération d'une doc doxygen</t>
+  </si>
+  <si>
+    <t>j'ai continué à faire la documentation</t>
+  </si>
+  <si>
+    <t>j'ai discuté avec le CdP et nous avons fait un bref point sur la documentation</t>
+  </si>
+  <si>
+    <t>j'ai regardé la solution pour communiqué par le réseau fournie par e CdP, mais cela ne correspond pas à mes besoins, car l'utilisateur doit lancer une commande sur le cmd pour pouvoir communiquer avec quelqu'un d'autre, je regarde une autre solution utilisant les sockets</t>
   </si>
 </sst>
 </file>
@@ -672,7 +681,7 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,315 +1623,348 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="1">
-        <f>SUM($D$3:$D73)</f>
-        <v>2.1319444444444446</v>
-      </c>
+      <c r="A73" s="12">
+        <v>43545</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E74" s="1">
         <f>SUM($D$3:$D74)</f>
-        <v>2.1319444444444446</v>
+        <v>2.1944444444444446</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E75" s="1">
-        <f>SUM($D$3:$D75)</f>
-        <v>2.1319444444444446</v>
-      </c>
+      <c r="A75" s="12">
+        <v>43546</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D76" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="E76" s="1">
         <f>SUM($D$3:$D76)</f>
-        <v>2.1319444444444446</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.2013888888888893</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D77" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
       <c r="E77" s="1">
         <f>SUM($D$3:$D77)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E78" s="1">
         <f>SUM($D$3:$D78)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E79" s="1">
         <f>SUM($D$3:$D79)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E80" s="1">
         <f>SUM($D$3:$D80)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="1">
         <f>SUM($D$3:$D81)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="1">
         <f>SUM($D$3:$D82)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="1">
         <f>SUM($D$3:$D83)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="1">
         <f>SUM($D$3:$D84)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="1">
         <f>SUM($D$3:$D85)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" s="1">
         <f>SUM($D$3:$D86)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" s="1">
         <f>SUM($D$3:$D87)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" s="1">
         <f>SUM($D$3:$D88)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" s="1">
         <f>SUM($D$3:$D89)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" s="1">
         <f>SUM($D$3:$D90)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" s="1">
         <f>SUM($D$3:$D91)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" s="1">
         <f>SUM($D$3:$D92)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" s="1">
         <f>SUM($D$3:$D93)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" s="1">
         <f>SUM($D$3:$D94)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" s="1">
         <f>SUM($D$3:$D95)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" s="1">
         <f>SUM($D$3:$D96)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="1">
         <f>SUM($D$3:$D97)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="1">
         <f>SUM($D$3:$D98)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="1">
         <f>SUM($D$3:$D99)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="1">
         <f>SUM($D$3:$D100)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="1">
         <f>SUM($D$3:$D101)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="1">
         <f>SUM($D$3:$D102)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="1">
         <f>SUM($D$3:$D103)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="1">
         <f>SUM($D$3:$D104)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="1">
         <f>SUM($D$3:$D105)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="1">
         <f>SUM($D$3:$D106)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="1">
         <f>SUM($D$3:$D107)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="1">
         <f>SUM($D$3:$D108)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="1">
         <f>SUM($D$3:$D109)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="1">
         <f>SUM($D$3:$D110)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="1">
         <f>SUM($D$3:$D111)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="1">
         <f>SUM($D$3:$D112)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="1">
         <f>SUM($D$3:$D113)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="1">
         <f>SUM($D$3:$D114)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="1">
         <f>SUM($D$3:$D115)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="1">
         <f>SUM($D$3:$D116)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="1">
         <f>SUM($D$3:$D117)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="1">
         <f>SUM($D$3:$D118)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="1">
         <f>SUM($D$3:$D119)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="1">
         <f>SUM($D$3:$D120)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="1">
         <f>SUM($D$3:$D121)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="1">
         <f>SUM($D$3:$D122)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="1">
         <f>SUM($D$3:$D123)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="1">
         <f>SUM($D$3:$D124)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
j'ai testé de communiquer sur un autre ordinateur et cela n'a pas fonctionné...
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,13 @@
   </si>
   <si>
     <t>resumé de rapport</t>
+  </si>
+  <si>
+    <t>j'ai créé l'interface demandant l'adresse ip de l'adversaire et j'essaie de faire que quand on met l'IP un test de connection est effectué.
+Actuellement je bloque sur les exception que cela génère.</t>
+  </si>
+  <si>
+    <t>tests sur l'implementation des sockets dans le projet, mais celui-ci me fait des erreur qui passent outre le try and catch</t>
   </si>
 </sst>
 </file>
@@ -689,8 +696,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="C67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1734,7 @@
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1749,7 @@
         <v>2.3506944444444446</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>5</v>
       </c>
@@ -1757,256 +1764,280 @@
         <v>2.3819444444444446</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="1">
-        <f>SUM($D$3:$D83)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="12">
+        <v>43551</v>
+      </c>
+      <c r="B83" s="12"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+    </row>
+    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E84" s="1">
         <f>SUM($D$3:$D84)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="1">
-        <f>SUM($D$3:$D85)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.4444444444444446</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="12">
+        <v>43552</v>
+      </c>
+      <c r="B85" s="12"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+    </row>
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D86" s="2">
+        <v>6.25E-2</v>
+      </c>
       <c r="E86" s="1">
         <f>SUM($D$3:$D86)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E87" s="1">
         <f>SUM($D$3:$D87)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E88" s="1">
         <f>SUM($D$3:$D88)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E89" s="1">
         <f>SUM($D$3:$D89)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E90" s="1">
         <f>SUM($D$3:$D90)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E91" s="1">
         <f>SUM($D$3:$D91)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E92" s="1">
         <f>SUM($D$3:$D92)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E93" s="1">
         <f>SUM($D$3:$D93)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E94" s="1">
         <f>SUM($D$3:$D94)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E95" s="1">
         <f>SUM($D$3:$D95)</f>
-        <v>2.3819444444444446</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+        <v>2.5069444444444446</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E96" s="1">
         <f>SUM($D$3:$D96)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" s="1">
         <f>SUM($D$3:$D97)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" s="1">
         <f>SUM($D$3:$D98)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" s="1">
         <f>SUM($D$3:$D99)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" s="1">
         <f>SUM($D$3:$D100)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" s="1">
         <f>SUM($D$3:$D101)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" s="1">
         <f>SUM($D$3:$D102)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="1">
         <f>SUM($D$3:$D103)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="1">
         <f>SUM($D$3:$D104)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="1">
         <f>SUM($D$3:$D105)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" s="1">
         <f>SUM($D$3:$D106)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" s="1">
         <f>SUM($D$3:$D107)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" s="1">
         <f>SUM($D$3:$D108)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" s="1">
         <f>SUM($D$3:$D109)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" s="1">
         <f>SUM($D$3:$D110)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" s="1">
         <f>SUM($D$3:$D111)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" s="1">
         <f>SUM($D$3:$D112)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="1">
         <f>SUM($D$3:$D113)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="1">
         <f>SUM($D$3:$D114)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="1">
         <f>SUM($D$3:$D115)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="1">
         <f>SUM($D$3:$D116)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="1">
         <f>SUM($D$3:$D117)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="1">
         <f>SUM($D$3:$D118)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="1">
         <f>SUM($D$3:$D119)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="1">
         <f>SUM($D$3:$D120)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="1">
         <f>SUM($D$3:$D121)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="1">
         <f>SUM($D$3:$D122)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="1">
         <f>SUM($D$3:$D123)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="1">
         <f>SUM($D$3:$D124)</f>
-        <v>2.3819444444444446</v>
+        <v>2.5069444444444446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentation et test des sockets
</commit_message>
<xml_diff>
--- a/journal de Travail.xlsx
+++ b/journal de Travail.xlsx
@@ -10,6 +10,9 @@
     <sheet name="Pre TPI" sheetId="1" r:id="rId1"/>
     <sheet name="Parametre" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -191,6 +194,27 @@
     <t>génération d'une doc doxygen</t>
   </si>
   <si>
+    <t xml:space="preserve">création du wireframe </t>
+  </si>
+  <si>
+    <t>mise en place de l'interface en fonction du wireframe</t>
+  </si>
+  <si>
+    <t>recherches de comment mettre en place le mvc en c#</t>
+  </si>
+  <si>
+    <t>mise en place de l'interface graphique en mvc</t>
+  </si>
+  <si>
+    <t>mise en place de classes test, création des IA facile, moyenne et difficile.</t>
+  </si>
+  <si>
+    <t>documentation des différents points</t>
+  </si>
+  <si>
+    <t>Mise en place de l'interface Informations, correction du code des bases de données</t>
+  </si>
+  <si>
     <t>j'ai continué à faire la documentation</t>
   </si>
   <si>
@@ -214,16 +238,35 @@
   </si>
   <si>
     <t>tests sur l'implementation des sockets dans le projet, mais celui-ci me fait des erreur qui passent outre le try and catch</t>
+  </si>
+  <si>
+    <t>malade</t>
+  </si>
+  <si>
+    <t>J'ai essayé de mettre un petit timer avant chaque coup de l'ordinateur, mais malheureusement le timer impacte aussi la pose du joueur…., je l'ai donc enlevé</t>
+  </si>
+  <si>
+    <t>mise en place du MVC réussie</t>
+  </si>
+  <si>
+    <t>problème dans l'historique de mon journal de travail, correction de celui-ci, j'avais mon journal en différé à cause des différentes branches.</t>
+  </si>
+  <si>
+    <t>correction de quelques petits points, plus ajout de mes recherches dans la documentation</t>
+  </si>
+  <si>
+    <t>j'arrive à envoyer mon socket en local, mais j'essaie de comprendre pourquoi mon code plante dès qu'il faut envoyer à un autre pc. Via telnet nous arrivons a communiquer avec le server</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[hh]:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,14 +277,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -275,35 +310,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -326,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -370,14 +381,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,16 +422,31 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Pre TPI"/>
+      <sheetName val="Parametre"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E124" totalsRowShown="0">
-  <autoFilter ref="A1:E124"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E121" totalsRowShown="0">
+  <autoFilter ref="A1:E121"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="4"/>
     <tableColumn id="5" name="Type" dataDxfId="3"/>
     <tableColumn id="2" name="Activité" dataDxfId="2"/>
     <tableColumn id="3" name="Temps" dataDxfId="1"/>
     <tableColumn id="4" name="Temps journée" dataDxfId="0">
-      <calculatedColumnFormula>SUM($D2:$D$124)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM($D2:$D$121)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
@@ -694,10 +717,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +732,7 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -726,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43500</v>
       </c>
@@ -734,136 +757,143 @@
       <c r="C2" s="9"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="11">
         <v>6.25E-2</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="18">
         <f>SUM($D$3:$D3)</f>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43501</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>3.125E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="18">
         <f>SUM($D$3:$D5)</f>
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43502</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="18">
+        <f>SUM($D$3:$D6)</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>4.8611111111111112E-2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="18">
         <f>SUM($D$3:$D7)</f>
         <v>0.1423611111111111</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="18">
         <f>SUM($D$3:$D8)</f>
         <v>0.15625</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43503</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="18">
+        <f>SUM($D$3:$D9)</f>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="18">
         <f>SUM($D$3:$D10)</f>
         <v>0.23958333333333331</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43504</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="18">
+        <f>SUM($D$3:$D11)</f>
+        <v>0.23958333333333331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="2">
         <v>3.125E-2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="18">
         <f>SUM($D$3:$D12)</f>
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
@@ -873,12 +903,12 @@
       <c r="D13" s="2">
         <v>3.125E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="18">
         <f>SUM($D$3:$D13)</f>
         <v>0.30208333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -888,21 +918,24 @@
       <c r="D14" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="18">
         <f>SUM($D$3:$D14)</f>
         <v>0.36458333333333331</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43507</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="18">
+        <f>SUM($D$3:$D15)</f>
+        <v>0.36458333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
@@ -912,7 +945,7 @@
       <c r="D16" s="2">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="18">
         <f>SUM($D$3:$D16)</f>
         <v>0.375</v>
       </c>
@@ -927,159 +960,174 @@
       <c r="D17" s="2">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="18">
         <f>SUM($D$3:$D17)</f>
         <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <v>43509</v>
+        <v>43508</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="E18" s="18">
+        <f>SUM($D$3:$D18)</f>
+        <v>0.42708333333333331</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E19" s="1">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="E19" s="18">
         <f>SUM($D$3:$D19)</f>
-        <v>0.45833333333333331</v>
+        <v>0.46527777777777773</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E20" s="1">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="E20" s="18">
         <f>SUM($D$3:$D20)</f>
         <v>0.48958333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
-        <v>43510</v>
+        <v>43509</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="E21" s="18">
+        <f>SUM($D$3:$D21)</f>
+        <v>0.48958333333333331</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2">
         <v>3.125E-2</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="18">
         <f>SUM($D$3:$D22)</f>
         <v>0.52083333333333326</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E23" s="18">
+        <f>SUM($D$3:$D23)</f>
+        <v>0.55208333333333326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>43510</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="18">
+        <f>SUM($D$3:$D24)</f>
+        <v>0.55208333333333326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E25" s="18">
+        <f>SUM($D$3:$D25)</f>
+        <v>0.58333333333333326</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <v>43511</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="18">
+        <f>SUM($D$3:$D26)</f>
+        <v>0.58333333333333326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D27" s="2">
         <v>0.17708333333333334</v>
       </c>
-      <c r="E24" s="1">
-        <f>SUM($D$3:$D24)</f>
-        <v>0.69791666666666663</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>43514</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E26" s="1">
-        <f>SUM($D$3:$D26)</f>
-        <v>0.71180555555555547</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="E27" s="18">
         <f>SUM($D$3:$D27)</f>
-        <v>0.7534722222222221</v>
+        <v>0.76041666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <v>43516</v>
+        <v>43514</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
       <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="E28" s="18">
+        <f>SUM($D$3:$D28)</f>
+        <v>0.76041666666666663</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E29" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E29" s="18">
         <f>SUM($D$3:$D29)</f>
-        <v>0.7847222222222221</v>
+        <v>0.77430555555555547</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1087,219 +1135,233 @@
         <v>7</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E30" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E30" s="18">
         <f>SUM($D$3:$D30)</f>
         <v>0.8159722222222221</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <v>43517</v>
+        <v>43515</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="E31" s="18">
+        <f>SUM($D$3:$D31)</f>
+        <v>0.8159722222222221</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E32" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E32" s="18">
         <f>SUM($D$3:$D32)</f>
+        <v>0.83680555555555547</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E33" s="18">
+        <f>SUM($D$3:$D33)</f>
         <v>0.8784722222222221</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>43528</v>
-      </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-    </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="A34" s="12">
+        <v>43516</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="18">
         <f>SUM($D$3:$D34)</f>
+        <v>0.8784722222222221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E35" s="18">
+        <f>SUM($D$3:$D35)</f>
+        <v>0.9097222222222221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E36" s="18">
+        <f>SUM($D$3:$D36)</f>
         <v>0.9409722222222221</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
-        <v>43529</v>
-      </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E36" s="1">
-        <f>SUM($D$3:$D36)</f>
-        <v>1.0034722222222221</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <v>43529</v>
+        <v>43517</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="13"/>
       <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
+      <c r="E37" s="18">
+        <f>SUM($D$3:$D37)</f>
+        <v>0.9409722222222221</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D38" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E38" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E38" s="18">
         <f>SUM($D$3:$D38)</f>
-        <v>1.0347222222222221</v>
+        <v>1.0034722222222221</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="A39" s="12">
+        <v>43518</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="18">
         <f>SUM($D$3:$D39)</f>
-        <v>1.0486111111111109</v>
-      </c>
-      <c r="F39" s="7"/>
+        <v>1.0034722222222221</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="D40" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E40" s="1">
+        <v>0.21875</v>
+      </c>
+      <c r="E40" s="18">
         <f>SUM($D$3:$D40)</f>
-        <v>1.0590277777777777</v>
+        <v>1.2222222222222221</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E41" s="1">
+      <c r="A41" s="12">
+        <v>43528</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="18">
         <f>SUM($D$3:$D41)</f>
-        <v>1.0659722222222221</v>
+        <v>1.2222222222222221</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
-        <v>43530</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
+      <c r="B42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E42" s="18">
+        <f>SUM($D$3:$D42)</f>
+        <v>1.2847222222222221</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E43" s="1">
+      <c r="A43" s="12">
+        <v>43529</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="18">
         <f>SUM($D$3:$D43)</f>
-        <v>1.0972222222222221</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.2847222222222221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D44" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="18">
         <f>SUM($D$3:$D44)</f>
-        <v>1.1597222222222221</v>
+        <v>1.3472222222222221</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <v>43531</v>
+        <v>43529</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="13"/>
       <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
+      <c r="E45" s="18">
+        <f>SUM($D$3:$D45)</f>
+        <v>1.3472222222222221</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D46" s="2">
-        <v>9.375E-2</v>
-      </c>
-      <c r="E46" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E46" s="18">
         <f>SUM($D$3:$D46)</f>
-        <v>1.2534722222222221</v>
+        <v>1.3784722222222221</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,92 +1369,99 @@
         <v>7</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D47" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E47" s="1">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E47" s="18">
         <f>SUM($D$3:$D47)</f>
-        <v>1.3159722222222221</v>
-      </c>
+        <v>1.3923611111111109</v>
+      </c>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D48" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E48" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E48" s="18">
         <f>SUM($D$3:$D48)</f>
-        <v>1.3784722222222221</v>
+        <v>1.4027777777777777</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="12">
-        <v>43533</v>
-      </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="B49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E49" s="18">
+        <f>SUM($D$3:$D49)</f>
+        <v>1.4097222222222221</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D50" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E50" s="1">
+      <c r="A50" s="12">
+        <v>43530</v>
+      </c>
+      <c r="B50" s="12"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="18">
         <f>SUM($D$3:$D50)</f>
-        <v>1.3993055555555554</v>
+        <v>1.4097222222222221</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D51" s="2">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="E51" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E51" s="18">
         <f>SUM($D$3:$D51)</f>
-        <v>1.4374999999999998</v>
+        <v>1.4409722222222221</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="12">
-        <v>43535</v>
-      </c>
-      <c r="B52" s="12"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
+      <c r="B52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E52" s="18">
+        <f>SUM($D$3:$D52)</f>
+        <v>1.5034722222222221</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D53" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E53" s="1">
+      <c r="A53" s="12">
+        <v>43531</v>
+      </c>
+      <c r="B53" s="12"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="18">
         <f>SUM($D$3:$D53)</f>
-        <v>1.4444444444444442</v>
+        <v>1.5034722222222221</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,14 +1469,14 @@
         <v>5</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D54" s="2">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="E54" s="1">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E54" s="18">
         <f>SUM($D$3:$D54)</f>
-        <v>1.4791666666666665</v>
+        <v>1.5972222222222221</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,391 +1484,436 @@
         <v>7</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D55" s="2">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E55" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E55" s="18">
         <f>SUM($D$3:$D55)</f>
-        <v>1.5069444444444442</v>
+        <v>1.6597222222222221</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="12">
-        <v>43536</v>
-      </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
+      <c r="B56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E56" s="18">
+        <f>SUM($D$3:$D56)</f>
+        <v>1.7222222222222221</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E57" s="1">
+      <c r="A57" s="12">
+        <v>43532</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="18">
         <f>SUM($D$3:$D57)</f>
-        <v>1.5694444444444442</v>
+        <v>1.7222222222222221</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="12">
-        <v>43537</v>
-      </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
+      <c r="B58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E58" s="18">
+        <f>SUM($D$3:$D58)</f>
+        <v>1.8472222222222221</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D59" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="18">
         <f>SUM($D$3:$D59)</f>
-        <v>1.6319444444444442</v>
+        <v>1.9097222222222221</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="12">
-        <v>43538</v>
-      </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
+      <c r="B60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E60" s="18">
+        <f>SUM($D$3:$D60)</f>
+        <v>1.9305555555555554</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D61" s="2">
-        <v>9.375E-2</v>
-      </c>
-      <c r="E61" s="1">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="E61" s="18">
         <f>SUM($D$3:$D61)</f>
-        <v>1.7256944444444442</v>
+        <v>1.9687499999999998</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
-        <v>43539</v>
+        <v>43535</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="13"/>
       <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
+      <c r="E62" s="18">
+        <f>SUM($D$3:$D62)</f>
+        <v>1.9687499999999998</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D63" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E63" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E63" s="18">
         <f>SUM($D$3:$D63)</f>
-        <v>1.9340277777777775</v>
+        <v>1.9756944444444442</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D64" s="2">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E64" s="1">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="E64" s="18">
         <f>SUM($D$3:$D64)</f>
-        <v>1.9444444444444442</v>
+        <v>2.0104166666666665</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="12">
-        <v>43541</v>
-      </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
+      <c r="B65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E65" s="18">
+        <f>SUM($D$3:$D65)</f>
+        <v>2.0381944444444442</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D66" s="2">
+      <c r="A66" s="12">
+        <v>43536</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="18">
+        <f>SUM($D$3:$D66)</f>
+        <v>2.0381944444444442</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E66" s="1">
-        <f>SUM($D$3:$D66)</f>
-        <v>2.0069444444444442</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="12">
-        <v>43542</v>
-      </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
+      <c r="E67" s="18">
+        <f>SUM($D$3:$D67)</f>
+        <v>2.1006944444444442</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D68" s="2">
+      <c r="A68" s="12">
+        <v>43537</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="18">
+        <f>SUM($D$3:$D68)</f>
+        <v>2.1006944444444442</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E68" s="1">
-        <f>SUM($D$3:$D68)</f>
-        <v>2.0694444444444442</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="12">
-        <v>43544</v>
-      </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
+      <c r="E69" s="18">
+        <f>SUM($D$3:$D69)</f>
+        <v>2.1631944444444442</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D70" s="2">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="E70" s="1">
+      <c r="A70" s="12">
+        <v>43538</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="18">
         <f>SUM($D$3:$D70)</f>
-        <v>2.0868055555555554</v>
+        <v>2.1631944444444442</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D71" s="2">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="E71" s="1">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E71" s="18">
         <f>SUM($D$3:$D71)</f>
-        <v>2.125</v>
+        <v>2.2569444444444442</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D72" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E72" s="1">
+      <c r="A72" s="12">
+        <v>43539</v>
+      </c>
+      <c r="B72" s="12"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="18">
         <f>SUM($D$3:$D72)</f>
-        <v>2.1319444444444446</v>
+        <v>2.2569444444444442</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="12">
-        <v>43545</v>
-      </c>
-      <c r="B73" s="12"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
+      <c r="B73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E73" s="18">
+        <f>SUM($D$3:$D73)</f>
+        <v>2.4652777777777777</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D74" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E74" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E74" s="18">
         <f>SUM($D$3:$D74)</f>
-        <v>2.1944444444444446</v>
+        <v>2.4756944444444442</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
-        <v>43546</v>
+        <v>43541</v>
       </c>
       <c r="B75" s="12"/>
       <c r="C75" s="13"/>
       <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
+      <c r="E75" s="18">
+        <f>SUM($D$3:$D75)</f>
+        <v>2.4756944444444442</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D76" s="2">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E76" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E76" s="18">
         <f>SUM($D$3:$D76)</f>
-        <v>2.2013888888888893</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D77" s="2">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E77" s="1">
+        <v>2.5381944444444442</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="12">
+        <v>43542</v>
+      </c>
+      <c r="B77" s="12"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="18">
         <f>SUM($D$3:$D77)</f>
-        <v>2.2569444444444446</v>
+        <v>2.5381944444444442</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="12">
-        <v>43549</v>
-      </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
+      <c r="B78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D78" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E78" s="18">
+        <f>SUM($D$3:$D78)</f>
+        <v>2.6006944444444442</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D79" s="2">
+      <c r="A79" s="12">
+        <v>43543</v>
+      </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="18">
+        <f>SUM($D$3:$D79)</f>
+        <v>2.6006944444444442</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E79" s="1">
-        <f>SUM($D$3:$D79)</f>
-        <v>2.3194444444444446</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="12">
-        <v>43550</v>
-      </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
+      <c r="E80" s="18">
+        <f>SUM($D$3:$D80)</f>
+        <v>2.6631944444444442</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C81" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E81" s="1">
+      <c r="A81" s="12">
+        <v>43544</v>
+      </c>
+      <c r="B81" s="12"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="18">
         <f>SUM($D$3:$D81)</f>
-        <v>2.3506944444444446</v>
+        <v>2.6631944444444442</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D82" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="E82" s="1">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E82" s="18">
         <f>SUM($D$3:$D82)</f>
-        <v>2.3819444444444446</v>
+        <v>2.6805555555555554</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="12">
-        <v>43551</v>
-      </c>
-      <c r="B83" s="12"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-    </row>
-    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D83" s="2">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="E83" s="18">
+        <f>SUM($D$3:$D83)</f>
+        <v>2.71875</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D84" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E84" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E84" s="18">
         <f>SUM($D$3:$D84)</f>
-        <v>2.4444444444444446</v>
+        <v>2.7256944444444446</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
-        <v>43552</v>
+        <v>43545</v>
       </c>
       <c r="B85" s="12"/>
       <c r="C85" s="13"/>
       <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-    </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E85" s="18">
+        <f>SUM($D$3:$D85)</f>
+        <v>2.7256944444444446</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>63</v>
@@ -1807,237 +1921,375 @@
       <c r="D86" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="18">
         <f>SUM($D$3:$D86)</f>
-        <v>2.5069444444444446</v>
+        <v>2.7881944444444446</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="1">
+      <c r="A87" s="12">
+        <v>43546</v>
+      </c>
+      <c r="B87" s="12"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="18">
         <f>SUM($D$3:$D87)</f>
-        <v>2.5069444444444446</v>
+        <v>2.7881944444444446</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="1">
+      <c r="B88" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D88" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E88" s="18">
         <f>SUM($D$3:$D88)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E89" s="1">
+        <v>2.7951388888888893</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D89" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E89" s="18">
         <f>SUM($D$3:$D89)</f>
-        <v>2.5069444444444446</v>
+        <v>2.8506944444444446</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E90" s="1">
+      <c r="A90" s="12">
+        <v>43549</v>
+      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="18">
         <f>SUM($D$3:$D90)</f>
-        <v>2.5069444444444446</v>
+        <v>2.8506944444444446</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="1">
+      <c r="B91" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D91" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E91" s="18">
         <f>SUM($D$3:$D91)</f>
-        <v>2.5069444444444446</v>
+        <v>2.9131944444444446</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E92" s="1">
+      <c r="A92" s="12">
+        <v>43550</v>
+      </c>
+      <c r="B92" s="12"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="18">
         <f>SUM($D$3:$D92)</f>
-        <v>2.5069444444444446</v>
+        <v>2.9131944444444446</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E93" s="1">
+      <c r="B93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D93" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E93" s="18">
         <f>SUM($D$3:$D93)</f>
-        <v>2.5069444444444446</v>
+        <v>2.9444444444444446</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E94" s="1">
+      <c r="B94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D94" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E94" s="18">
         <f>SUM($D$3:$D94)</f>
-        <v>2.5069444444444446</v>
+        <v>2.9756944444444446</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="1">
+      <c r="A95" s="12">
+        <v>43551</v>
+      </c>
+      <c r="B95" s="12"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="18">
         <f>SUM($D$3:$D95)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E96" s="1">
+        <v>2.9756944444444446</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B96" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D96" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E96" s="18">
         <f>SUM($D$3:$D96)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="1">
+        <v>3.0381944444444446</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="12">
+        <v>43552</v>
+      </c>
+      <c r="B97" s="12"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="18">
         <f>SUM($D$3:$D97)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" s="1">
+        <v>3.0381944444444446</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B98" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" s="2">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E98" s="18">
         <f>SUM($D$3:$D98)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" s="1">
+        <v>3.1319444444444446</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="12">
+        <v>43553</v>
+      </c>
+      <c r="B99" s="12"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="18">
         <f>SUM($D$3:$D99)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" s="1">
+        <v>3.1319444444444446</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.21875</v>
+      </c>
+      <c r="E100" s="18">
         <f>SUM($D$3:$D100)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" s="1">
+        <v>3.3506944444444446</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="12">
+        <v>43556</v>
+      </c>
+      <c r="B101" s="12"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="18">
         <f>SUM($D$3:$D101)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" s="1">
+        <v>3.3506944444444446</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D102" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E102" s="18">
         <f>SUM($D$3:$D102)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" s="1">
+        <v>3.3819444444444446</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="12">
+        <v>43557</v>
+      </c>
+      <c r="B103" s="12"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="18">
         <f>SUM($D$3:$D103)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" s="1">
+        <v>3.3819444444444446</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D104" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E104" s="18">
         <f>SUM($D$3:$D104)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" s="1">
+        <v>3.3958333333333335</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D105" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E105" s="18">
         <f>SUM($D$3:$D105)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="1">
+        <v>3.4097222222222223</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D106" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E106" s="18">
         <f>SUM($D$3:$D106)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E107" s="1">
+        <v>3.4513888888888888</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="18">
         <f>SUM($D$3:$D107)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E108" s="1">
+        <v>3.4513888888888888</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="18">
         <f>SUM($D$3:$D108)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E109" s="1">
+        <v>3.4513888888888888</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="18">
         <f>SUM($D$3:$D109)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E110" s="1">
+        <v>3.4513888888888888</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="18">
         <f>SUM($D$3:$D110)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E111" s="1">
+        <v>3.4513888888888888</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="18">
         <f>SUM($D$3:$D111)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E112" s="1">
+        <v>3.4513888888888888</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="18">
         <f>SUM($D$3:$D112)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="1">
+      <c r="E113" s="18">
         <f>SUM($D$3:$D113)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="1">
+      <c r="E114" s="18">
         <f>SUM($D$3:$D114)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E115" s="1">
+      <c r="E115" s="18">
         <f>SUM($D$3:$D115)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E116" s="1">
+      <c r="E116" s="18">
         <f>SUM($D$3:$D116)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E117" s="1">
+      <c r="E117" s="18">
         <f>SUM($D$3:$D117)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E118" s="1">
+      <c r="E118" s="18">
         <f>SUM($D$3:$D118)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E119" s="1">
+      <c r="E119" s="18">
         <f>SUM($D$3:$D119)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E120" s="1">
+      <c r="E120" s="18">
         <f>SUM($D$3:$D120)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E121" s="1">
+      <c r="E121" s="18">
         <f>SUM($D$3:$D121)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E122" s="1">
-        <f>SUM($D$3:$D122)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E123" s="1">
-        <f>SUM($D$3:$D123)</f>
-        <v>2.5069444444444446</v>
-      </c>
-    </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E124" s="1">
-        <f>SUM($D$3:$D124)</f>
-        <v>2.5069444444444446</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
   </sheetData>
@@ -2048,12 +2300,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametre!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B2946</xm:sqref>
+          <xm:sqref>B2:B18 B60:B84 B96 B86 B88:B89 B91 B93:B94 B98 B100 B21:B57 B102 B104:B2943</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[journal de Travail3.xlsx]Parametre'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B85 B87 B90 B92 B95 B97 B99 B101 B103</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>